<commit_message>
Completed HW 2/26 - Desktop
</commit_message>
<xml_diff>
--- a/DataBase Files/test/Session 28 tables.xlsx
+++ b/DataBase Files/test/Session 28 tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shain\repos\Recipe-Apps\DataBase Files\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E518983F-105B-4171-AE2F-CE5246EA10DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF15F46F-D61F-4BA9-A5E3-A6E80896B807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3BB324A-D888-47B0-B036-72B9FE8204B1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -986,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166C56E4-FA94-4162-A9C1-750288E7F497}">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>